<commit_message>
bug fixed, css and testcases update
</commit_message>
<xml_diff>
--- a/assets/testing/rev03_testcases.xlsx
+++ b/assets/testing/rev03_testcases.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="210">
   <si>
     <t>No.</t>
   </si>
@@ -667,22 +667,13 @@
     <t>1. Click "Look at me!" text</t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>1. Watch the webpage on 576 px</t>
   </si>
   <si>
     <t>2020.04.07</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>576 px issue</t>
-  </si>
-  <si>
-    <t>allgoods.html, dalahorsegoods.html, roostergoods.html - Resolution = 576px : the goods images have problem for the sizes, refer [Bugs capture] - 576px issue</t>
   </si>
   <si>
     <r>
@@ -703,10 +694,16 @@
     </r>
   </si>
   <si>
-    <t>Same as above</t>
-  </si>
-  <si>
     <t>Responsive &amp; Browser test</t>
+  </si>
+  <si>
+    <t>2020.04.09</t>
+  </si>
+  <si>
+    <t>CSS : Media query value was wrong. ".card img" 576.02px -&gt; 575.98px</t>
+  </si>
+  <si>
+    <t>Refer [Bugs capture] sheet : 576 px issue</t>
   </si>
 </sst>
 </file>
@@ -824,7 +821,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,14 +882,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="65">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -1521,21 +1512,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1738,7 +1714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1888,22 +1864,19 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1919,8 +1892,50 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2003,22 +2018,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2059,213 +2074,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -2798,7 +2612,7 @@
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:E4"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2822,64 +2636,64 @@
       <c r="J1" s="9"/>
     </row>
     <row r="2" spans="2:14" ht="18">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="71" t="s">
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="84" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15.6" customHeight="1">
-      <c r="B3" s="83"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="85" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="80" t="s">
+      <c r="I3" s="94"/>
+      <c r="J3" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="81"/>
-      <c r="L3" s="80" t="s">
+      <c r="K3" s="94"/>
+      <c r="L3" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="81"/>
-      <c r="N3" s="72"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B4" s="84"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
       <c r="H4" s="26" t="s">
         <v>62</v>
       </c>
@@ -2898,7 +2712,7 @@
       <c r="M4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="73"/>
+      <c r="N4" s="86"/>
     </row>
     <row r="5" spans="2:14" ht="58.2" thickTop="1">
       <c r="B5" s="5">
@@ -2943,7 +2757,7 @@
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="81" t="s">
         <v>139</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2982,7 +2796,7 @@
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="69"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3019,7 +2833,7 @@
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="69"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="3" t="s">
         <v>141</v>
       </c>
@@ -3056,7 +2870,7 @@
       <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="3" t="s">
         <v>142</v>
       </c>
@@ -3093,7 +2907,7 @@
       <c r="B10" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="3" t="s">
         <v>143</v>
       </c>
@@ -3130,7 +2944,7 @@
       <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="3" t="s">
         <v>144</v>
       </c>
@@ -3167,7 +2981,7 @@
       <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="69"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
@@ -3204,7 +3018,7 @@
       <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="69"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -3241,7 +3055,7 @@
       <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="3" t="s">
         <v>145</v>
       </c>
@@ -3278,7 +3092,7 @@
       <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="69"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
@@ -3315,7 +3129,7 @@
       <c r="B16" s="5">
         <v>12</v>
       </c>
-      <c r="C16" s="69"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
@@ -3352,7 +3166,7 @@
       <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="69"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
@@ -3389,7 +3203,7 @@
       <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" s="69"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
@@ -3426,7 +3240,7 @@
       <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="70"/>
+      <c r="C19" s="83"/>
       <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
@@ -3463,13 +3277,13 @@
       <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="C20" s="68" t="s">
+      <c r="C20" s="81" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="78" t="s">
         <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
@@ -3502,11 +3316,11 @@
       <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" s="69"/>
+      <c r="C21" s="82"/>
       <c r="D21" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E21" s="66"/>
+      <c r="E21" s="79"/>
       <c r="F21" s="6" t="s">
         <v>55</v>
       </c>
@@ -3537,11 +3351,11 @@
       <c r="B22" s="5">
         <v>18</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="83"/>
       <c r="D22" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E22" s="67"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="6" t="s">
         <v>55</v>
       </c>
@@ -3572,7 +3386,7 @@
       <c r="B23" s="5">
         <v>19</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="81" t="s">
         <v>149</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -3611,7 +3425,7 @@
       <c r="B24" s="5">
         <v>20</v>
       </c>
-      <c r="C24" s="69"/>
+      <c r="C24" s="82"/>
       <c r="D24" s="3" t="s">
         <v>35</v>
       </c>
@@ -3648,7 +3462,7 @@
       <c r="B25" s="5">
         <v>21</v>
       </c>
-      <c r="C25" s="69"/>
+      <c r="C25" s="82"/>
       <c r="D25" s="3" t="s">
         <v>33</v>
       </c>
@@ -3685,7 +3499,7 @@
       <c r="B26" s="5">
         <v>22</v>
       </c>
-      <c r="C26" s="70"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="3" t="s">
         <v>34</v>
       </c>
@@ -3722,7 +3536,7 @@
       <c r="B27" s="5">
         <v>23</v>
       </c>
-      <c r="C27" s="68" t="s">
+      <c r="C27" s="81" t="s">
         <v>150</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -3761,7 +3575,7 @@
       <c r="B28" s="5">
         <v>24</v>
       </c>
-      <c r="C28" s="69"/>
+      <c r="C28" s="82"/>
       <c r="D28" s="3" t="s">
         <v>35</v>
       </c>
@@ -3798,7 +3612,7 @@
       <c r="B29" s="5">
         <v>25</v>
       </c>
-      <c r="C29" s="69"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="3" t="s">
         <v>36</v>
       </c>
@@ -3835,7 +3649,7 @@
       <c r="B30" s="5">
         <v>26</v>
       </c>
-      <c r="C30" s="68" t="s">
+      <c r="C30" s="81" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -3874,7 +3688,7 @@
       <c r="B31" s="5">
         <v>27</v>
       </c>
-      <c r="C31" s="69"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="3" t="s">
         <v>35</v>
       </c>
@@ -3911,7 +3725,7 @@
       <c r="B32" s="5">
         <v>28</v>
       </c>
-      <c r="C32" s="69"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="3" t="s">
         <v>36</v>
       </c>
@@ -3948,7 +3762,7 @@
       <c r="B33" s="5">
         <v>29</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="81" t="s">
         <v>38</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -3987,7 +3801,7 @@
       <c r="B34" s="5">
         <v>30</v>
       </c>
-      <c r="C34" s="69"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="3" t="s">
         <v>35</v>
       </c>
@@ -4024,7 +3838,7 @@
       <c r="B35" s="5">
         <v>31</v>
       </c>
-      <c r="C35" s="68" t="s">
+      <c r="C35" s="81" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -4063,7 +3877,7 @@
       <c r="B36" s="5">
         <v>32</v>
       </c>
-      <c r="C36" s="69"/>
+      <c r="C36" s="82"/>
       <c r="D36" s="3" t="s">
         <v>71</v>
       </c>
@@ -4100,7 +3914,7 @@
       <c r="B37" s="5">
         <v>33</v>
       </c>
-      <c r="C37" s="70"/>
+      <c r="C37" s="83"/>
       <c r="D37" s="3" t="s">
         <v>35</v>
       </c>
@@ -4137,7 +3951,7 @@
       <c r="B38" s="5">
         <v>34</v>
       </c>
-      <c r="C38" s="68" t="s">
+      <c r="C38" s="81" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -4176,7 +3990,7 @@
       <c r="B39" s="5">
         <v>35</v>
       </c>
-      <c r="C39" s="69"/>
+      <c r="C39" s="82"/>
       <c r="D39" s="3" t="s">
         <v>42</v>
       </c>
@@ -4213,7 +4027,7 @@
       <c r="B40" s="5">
         <v>36</v>
       </c>
-      <c r="C40" s="69"/>
+      <c r="C40" s="82"/>
       <c r="D40" s="3" t="s">
         <v>35</v>
       </c>
@@ -4250,7 +4064,7 @@
       <c r="B41" s="5">
         <v>37</v>
       </c>
-      <c r="C41" s="70"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="3" t="s">
         <v>46</v>
       </c>
@@ -4287,7 +4101,7 @@
       <c r="B42" s="5">
         <v>38</v>
       </c>
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="81" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -4326,7 +4140,7 @@
       <c r="B43" s="5">
         <v>39</v>
       </c>
-      <c r="C43" s="69"/>
+      <c r="C43" s="82"/>
       <c r="D43" s="3" t="s">
         <v>42</v>
       </c>
@@ -4363,7 +4177,7 @@
       <c r="B44" s="5">
         <v>40</v>
       </c>
-      <c r="C44" s="69"/>
+      <c r="C44" s="82"/>
       <c r="D44" s="3" t="s">
         <v>35</v>
       </c>
@@ -4400,7 +4214,7 @@
       <c r="B45" s="5">
         <v>41</v>
       </c>
-      <c r="C45" s="70"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="3" t="s">
         <v>46</v>
       </c>
@@ -4437,7 +4251,7 @@
       <c r="B46" s="5">
         <v>46</v>
       </c>
-      <c r="C46" s="68" t="s">
+      <c r="C46" s="81" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -4476,7 +4290,7 @@
       <c r="B47" s="5">
         <v>47</v>
       </c>
-      <c r="C47" s="69"/>
+      <c r="C47" s="82"/>
       <c r="D47" s="3" t="s">
         <v>35</v>
       </c>
@@ -4513,7 +4327,7 @@
       <c r="B48" s="5">
         <v>48</v>
       </c>
-      <c r="C48" s="69"/>
+      <c r="C48" s="82"/>
       <c r="D48" s="3" t="s">
         <v>50</v>
       </c>
@@ -4550,7 +4364,7 @@
       <c r="B49" s="5">
         <v>49</v>
       </c>
-      <c r="C49" s="70"/>
+      <c r="C49" s="83"/>
       <c r="D49" s="3" t="s">
         <v>51</v>
       </c>
@@ -4587,7 +4401,7 @@
       <c r="B50" s="5">
         <v>50</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="81" t="s">
         <v>53</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -4626,7 +4440,7 @@
       <c r="B51" s="5">
         <v>51</v>
       </c>
-      <c r="C51" s="69"/>
+      <c r="C51" s="82"/>
       <c r="D51" s="3" t="s">
         <v>77</v>
       </c>
@@ -4663,7 +4477,7 @@
       <c r="B52" s="5">
         <v>52</v>
       </c>
-      <c r="C52" s="69"/>
+      <c r="C52" s="82"/>
       <c r="D52" s="3" t="s">
         <v>79</v>
       </c>
@@ -4700,7 +4514,7 @@
       <c r="B53" s="5">
         <v>53</v>
       </c>
-      <c r="C53" s="69"/>
+      <c r="C53" s="82"/>
       <c r="D53" s="3" t="s">
         <v>81</v>
       </c>
@@ -4737,7 +4551,7 @@
       <c r="B54" s="5">
         <v>54</v>
       </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="83"/>
       <c r="D54" s="3" t="s">
         <v>83</v>
       </c>
@@ -4771,7 +4585,7 @@
       <c r="N54" s="1"/>
     </row>
     <row r="55" spans="2:14" ht="187.8" thickBot="1">
-      <c r="B55" s="111">
+      <c r="B55" s="64">
         <v>55</v>
       </c>
       <c r="C55" s="25" t="s">
@@ -4836,13 +4650,13 @@
     <mergeCell ref="L3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:M55">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4856,7 +4670,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4864,208 +4678,198 @@
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
     <col min="2" max="2" width="28.109375" customWidth="1"/>
     <col min="3" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="72.109375" customWidth="1"/>
+    <col min="8" max="8" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="23.4">
       <c r="B1" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B2" s="95" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="B2" s="108" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="2:8" ht="23.4" customHeight="1">
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1" thickBot="1">
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1">
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="111" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="87" t="s">
+      <c r="G6" s="100" t="s">
         <v>200</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="102" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.6" customHeight="1">
-      <c r="B7" s="93"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="90"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B8" s="94"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="91"/>
-    </row>
-    <row r="9" spans="2:8" ht="29.4" thickTop="1">
-      <c r="B9" s="62" t="s">
+      <c r="B8" s="107"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="104"/>
+    </row>
+    <row r="9" spans="2:8" ht="30" customHeight="1" thickTop="1">
+      <c r="B9" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" s="116" t="s">
-        <v>207</v>
-      </c>
+      <c r="C9" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="67"/>
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1">
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="120" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="116" t="s">
-        <v>209</v>
-      </c>
+      <c r="C10" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="67"/>
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1">
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="121" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="116" t="s">
-        <v>209</v>
-      </c>
+      <c r="C11" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="67"/>
     </row>
     <row r="12" spans="2:8" ht="30" customHeight="1">
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="122" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="119" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="116" t="s">
-        <v>209</v>
-      </c>
+      <c r="C12" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="67"/>
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" thickBot="1">
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="123" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="124" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="124" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="125" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="125" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="117" t="s">
-        <v>209</v>
-      </c>
+      <c r="C13" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5088,7 +4892,7 @@
   <dimension ref="B1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5236,7 +5040,7 @@
       <c r="J3" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="K3" s="114" t="s">
+      <c r="K3" s="66" t="s">
         <v>160</v>
       </c>
       <c r="L3" s="31" t="s">
@@ -5262,8 +5066,8 @@
       <c r="B4" s="35">
         <v>3</v>
       </c>
-      <c r="C4" s="112" t="s">
-        <v>202</v>
+      <c r="C4" s="29" t="s">
+        <v>153</v>
       </c>
       <c r="D4" s="35" t="s">
         <v>161</v>
@@ -5286,7 +5090,7 @@
       <c r="J4" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="K4" s="113" t="s">
+      <c r="K4" s="65" t="s">
         <v>168</v>
       </c>
       <c r="L4" s="36" t="s">
@@ -5296,7 +5100,7 @@
         <v>165</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O4" s="38" t="s">
         <v>166</v>
@@ -5312,11 +5116,11 @@
       <c r="B5" s="35">
         <v>4</v>
       </c>
-      <c r="C5" s="115" t="s">
-        <v>205</v>
+      <c r="C5" s="29" t="s">
+        <v>153</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>56</v>
@@ -5328,7 +5132,7 @@
         <v>56</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>163</v>
@@ -5336,21 +5140,27 @@
       <c r="J5" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="K5" s="113" t="s">
-        <v>168</v>
+      <c r="K5" s="65" t="s">
+        <v>209</v>
       </c>
       <c r="L5" s="36" t="s">
         <v>130</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="N5" s="35"/>
-      <c r="O5" s="38"/>
+        <v>203</v>
+      </c>
+      <c r="N5" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>208</v>
+      </c>
       <c r="P5" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="Q5" s="35"/>
+      <c r="Q5" s="34" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5363,7 +5173,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5384,7 +5194,7 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -5398,7 +5208,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5411,102 +5221,102 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickTop="1">
       <c r="A1"/>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="101"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="114"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2"/>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="117"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3"/>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4"/>
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="115" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="104"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="117"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:7" ht="15.6">
       <c r="A5"/>
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="121" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="123"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6"/>
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="117"/>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7"/>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="117"/>
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8"/>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
       <c r="F8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="104"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="117"/>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1">
       <c r="A10"/>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
-      <c r="E10" s="107"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="120"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:7" ht="15.6" thickTop="1" thickBot="1">
@@ -5519,12 +5329,12 @@
     </row>
     <row r="12" spans="1:7" ht="24.6" thickTop="1" thickBot="1">
       <c r="A12"/>
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="114"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1">
@@ -5667,15 +5477,15 @@
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1"/>
     <row r="21" spans="2:7" ht="24.6" thickTop="1" thickBot="1">
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="101"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="114"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" thickBot="1">
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="77" t="s">
         <v>90</v>
       </c>
       <c r="C22" s="46" t="s">
@@ -5684,7 +5494,7 @@
       <c r="D22" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="53" t="s">
         <v>87</v>
       </c>
     </row>
@@ -5698,7 +5508,7 @@
       <c r="D23" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="54" t="s">
         <v>92</v>
       </c>
     </row>
@@ -5706,7 +5516,7 @@
       <c r="B24" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="56" t="s">
         <v>189</v>
       </c>
       <c r="D24" s="24" t="s">
@@ -5720,7 +5530,7 @@
       <c r="B25" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="56" t="s">
         <v>191</v>
       </c>
       <c r="D25" s="24" t="s">
@@ -5734,7 +5544,7 @@
       <c r="B26" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="56" t="s">
         <v>192</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -5745,10 +5555,10 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" thickBot="1">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="57" t="s">
         <v>193</v>
       </c>
       <c r="D27" s="25" t="s">

</xml_diff>